<commit_message>
added next version and support material
</commit_message>
<xml_diff>
--- a/plug-ins/control/RedPitaya-Support/McBSP-Link-Hardware/MK3-RP-Link/mk3-shield-PCBWay-BOM.xlsx
+++ b/plug-ins/control/RedPitaya-Support/McBSP-Link-Hardware/MK3-RP-Link/mk3-shield-PCBWay-BOM.xlsx
@@ -22,12 +22,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="45">
   <si>
     <t xml:space="preserve">Percy Zahl, GXSM RP PACPLL Interface Project</t>
   </si>
   <si>
-    <t xml:space="preserve">MK3-SHIELD   BOM  (Bill of Materials)  PCB: 60x52mm</t>
+    <t xml:space="preserve">MK3-SHIELD   BOM  (Bill of Materials)  PCB: 60x60mm</t>
   </si>
   <si>
     <t xml:space="preserve">Date: 20210205</t>
@@ -200,6 +200,9 @@
     <t xml:space="preserve">Through Hole</t>
   </si>
   <si>
+    <t xml:space="preserve">5**</t>
+  </si>
+  <si>
     <t xml:space="preserve">JP1</t>
   </si>
   <si>
@@ -210,6 +213,30 @@
   </si>
   <si>
     <t xml:space="preserve">do not populate (development/testing only)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JP4/6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SamTec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESQ-122-13-L-T</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3row 44pos in two 2x 3x22 ESQ-122-13-L-T stacking board inter connect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">do not populate (bottom side mount!!)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DO NOT ORDER, INCLUDE AND  INSTALL!!!</t>
   </si>
 </sst>
 </file>
@@ -503,10 +530,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:I26"/>
+  <dimension ref="A2:I35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I10" activeCellId="0" sqref="I10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G2" activeCellId="0" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -687,44 +714,60 @@
       <c r="I10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6" t="n">
-        <v>5</v>
+      <c r="A11" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C11" s="6" t="n">
         <v>0</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="8" t="s">
         <v>34</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>33</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>31</v>
       </c>
       <c r="I11" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-      <c r="B12" s="7"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="8"/>
+      <c r="A12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" s="12"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
+      <c r="H12" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6"/>
@@ -738,8 +781,12 @@
       <c r="I13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
+      <c r="A14" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>44</v>
+      </c>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
@@ -836,7 +883,7 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
     </row>
-    <row r="25" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="13"/>
       <c r="B25" s="13"/>
       <c r="C25" s="13"/>
@@ -858,12 +905,44 @@
       <c r="H26" s="14"/>
       <c r="I26" s="14"/>
     </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="7"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A2:B3"/>
     <mergeCell ref="D2:F4"/>
     <mergeCell ref="A24:I24"/>
     <mergeCell ref="A26:I26"/>
+    <mergeCell ref="D27:F29"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.699305555555555" right="0.699305555555555" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -882,7 +961,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -905,7 +984,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>